<commit_message>
enlarged country langs table
</commit_message>
<xml_diff>
--- a/analysis/paper-2013-10/si-table7-lang-by-country/si-table7-lang-by-country-modified.xlsx
+++ b/analysis/paper-2013-10/si-table7-lang-by-country/si-table7-lang-by-country-modified.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="si-table7-lang-by-country-modif" sheetId="1" r:id="rId1"/>
+    <sheet name="si-table7-lang-by-country-lrg-1" sheetId="2" r:id="rId2"/>
+    <sheet name="si-table7-lang-by-country-lrg2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'si-table7-lang-by-country-lrg-1'!$C$2:$C$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'si-table7-lang-by-country-lrg2'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'si-table7-lang-by-country-modif'!$C$2:$C$173</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="356">
   <si>
     <t>Bangladesh</t>
   </si>
@@ -1096,7 +1100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1128,6 +1132,17 @@
     <font>
       <b/>
       <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
@@ -1178,7 +1193,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1298,8 +1313,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1327,8 +1358,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1388,6 +1445,14 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1447,9 +1512,1086 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1498,6 +2640,96 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
@@ -1526,6 +2758,96 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
@@ -1554,6 +2876,96 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
@@ -1582,6 +2994,96 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
@@ -1610,6 +3112,96 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
@@ -1638,6 +3230,96 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thick">
           <color theme="0"/>
@@ -1683,9 +3365,6 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1704,14 +3383,11 @@
         <name val="Times New Roman"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1729,7 +3405,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1766,618 +3442,6 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -2417,32 +3481,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:X26" headerRowCount="0" totalsRowShown="0" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:X26" headerRowCount="0" totalsRowShown="0" dataDxfId="100">
   <tableColumns count="24">
-    <tableColumn id="1" name=" " headerRowDxfId="29" dataDxfId="48"/>
-    <tableColumn id="2" name="Country" headerRowDxfId="30" dataDxfId="47"/>
-    <tableColumn id="3" name="Languages" headerRowDxfId="31" dataDxfId="7"/>
-    <tableColumn id="13" name="Column2" headerRowDxfId="28" dataDxfId="6"/>
-    <tableColumn id="14" name="Column3" headerRowDxfId="27" dataDxfId="25"/>
-    <tableColumn id="15" name="Column4" headerRowDxfId="26" dataDxfId="24"/>
-    <tableColumn id="4" name=" 2" headerRowDxfId="32" dataDxfId="5"/>
-    <tableColumn id="5" name="Country3" headerRowDxfId="33" dataDxfId="46"/>
-    <tableColumn id="6" name="Languages4" headerRowDxfId="34" dataDxfId="45"/>
-    <tableColumn id="16" name="Column5" headerRowDxfId="23" dataDxfId="4"/>
-    <tableColumn id="17" name="Column6" headerRowDxfId="22" dataDxfId="20"/>
-    <tableColumn id="18" name="Column7" headerRowDxfId="21" dataDxfId="19"/>
-    <tableColumn id="7" name="Column1" headerRowDxfId="35" dataDxfId="3"/>
-    <tableColumn id="8" name="Country5" headerRowDxfId="36" dataDxfId="44"/>
-    <tableColumn id="9" name="Languages6" headerRowDxfId="37" dataDxfId="43"/>
-    <tableColumn id="19" name="Column8" headerRowDxfId="18" dataDxfId="2"/>
-    <tableColumn id="20" name="Column9" headerRowDxfId="17" dataDxfId="15"/>
-    <tableColumn id="21" name="Column10" headerRowDxfId="16" dataDxfId="14"/>
-    <tableColumn id="10" name=" 3" headerRowDxfId="38" dataDxfId="1"/>
-    <tableColumn id="11" name="Country7" headerRowDxfId="39" dataDxfId="42"/>
-    <tableColumn id="12" name="Languages8" headerRowDxfId="40" dataDxfId="10"/>
-    <tableColumn id="22" name="Column11" headerRowDxfId="13" dataDxfId="0"/>
-    <tableColumn id="23" name="Column12" headerRowDxfId="12" dataDxfId="9"/>
-    <tableColumn id="24" name="Column13" headerRowDxfId="11" dataDxfId="8"/>
+    <tableColumn id="1" name=" " headerRowDxfId="99" dataDxfId="98"/>
+    <tableColumn id="2" name="Country" headerRowDxfId="97" dataDxfId="96"/>
+    <tableColumn id="3" name="Languages" headerRowDxfId="95" dataDxfId="94"/>
+    <tableColumn id="13" name="Column2" headerRowDxfId="93" dataDxfId="92"/>
+    <tableColumn id="14" name="Column3" headerRowDxfId="91" dataDxfId="90"/>
+    <tableColumn id="15" name="Column4" headerRowDxfId="89" dataDxfId="88"/>
+    <tableColumn id="4" name=" 2" headerRowDxfId="87" dataDxfId="86"/>
+    <tableColumn id="5" name="Country3" headerRowDxfId="85" dataDxfId="84"/>
+    <tableColumn id="6" name="Languages4" headerRowDxfId="83" dataDxfId="82"/>
+    <tableColumn id="16" name="Column5" headerRowDxfId="81" dataDxfId="80"/>
+    <tableColumn id="17" name="Column6" headerRowDxfId="79" dataDxfId="78"/>
+    <tableColumn id="18" name="Column7" headerRowDxfId="77" dataDxfId="76"/>
+    <tableColumn id="7" name="Column1" headerRowDxfId="75" dataDxfId="74"/>
+    <tableColumn id="8" name="Country5" headerRowDxfId="73" dataDxfId="72"/>
+    <tableColumn id="9" name="Languages6" headerRowDxfId="71" dataDxfId="70"/>
+    <tableColumn id="19" name="Column8" headerRowDxfId="69" dataDxfId="68"/>
+    <tableColumn id="20" name="Column9" headerRowDxfId="67" dataDxfId="66"/>
+    <tableColumn id="21" name="Column10" headerRowDxfId="65" dataDxfId="64"/>
+    <tableColumn id="10" name=" 3" headerRowDxfId="63" dataDxfId="62"/>
+    <tableColumn id="11" name="Country7" headerRowDxfId="61" dataDxfId="60"/>
+    <tableColumn id="12" name="Languages8" headerRowDxfId="59" dataDxfId="58"/>
+    <tableColumn id="22" name="Column11" headerRowDxfId="57" dataDxfId="56"/>
+    <tableColumn id="23" name="Column12" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="24" name="Column13" headerRowDxfId="53" dataDxfId="52"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table32" displayName="Table32" ref="A2:L26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <tableColumns count="12">
+    <tableColumn id="1" name=" " headerRowDxfId="51" dataDxfId="13"/>
+    <tableColumn id="2" name="Country" headerRowDxfId="50" dataDxfId="12"/>
+    <tableColumn id="3" name="Languages" headerRowDxfId="49" dataDxfId="11"/>
+    <tableColumn id="13" name="Column2" headerRowDxfId="48" dataDxfId="10"/>
+    <tableColumn id="14" name="Column3" headerRowDxfId="47" dataDxfId="9"/>
+    <tableColumn id="15" name="Column4" headerRowDxfId="46" dataDxfId="8"/>
+    <tableColumn id="4" name=" 2" headerRowDxfId="45" dataDxfId="7"/>
+    <tableColumn id="5" name="Country3" headerRowDxfId="44" dataDxfId="6"/>
+    <tableColumn id="6" name="Languages4" headerRowDxfId="43" dataDxfId="5"/>
+    <tableColumn id="16" name="Column5" headerRowDxfId="42" dataDxfId="4"/>
+    <tableColumn id="17" name="Column6" headerRowDxfId="41" dataDxfId="3"/>
+    <tableColumn id="18" name="Column7" headerRowDxfId="40" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table323" displayName="Table323" ref="A2:L26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <tableColumns count="12">
+    <tableColumn id="7" name="Column1" headerRowDxfId="39" dataDxfId="27"/>
+    <tableColumn id="8" name="Country5" headerRowDxfId="38" dataDxfId="26"/>
+    <tableColumn id="9" name="Languages6" headerRowDxfId="37" dataDxfId="25"/>
+    <tableColumn id="19" name="Column8" headerRowDxfId="36" dataDxfId="24"/>
+    <tableColumn id="20" name="Column9" headerRowDxfId="35" dataDxfId="23"/>
+    <tableColumn id="21" name="Column10" headerRowDxfId="34" dataDxfId="22"/>
+    <tableColumn id="10" name=" 3" headerRowDxfId="33" dataDxfId="21"/>
+    <tableColumn id="11" name="Country7" headerRowDxfId="32" dataDxfId="20"/>
+    <tableColumn id="12" name="Languages8" headerRowDxfId="31" dataDxfId="19"/>
+    <tableColumn id="22" name="Column11" headerRowDxfId="30" dataDxfId="18"/>
+    <tableColumn id="23" name="Column12" headerRowDxfId="29" dataDxfId="17"/>
+    <tableColumn id="24" name="Column13" headerRowDxfId="28" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2772,8 +3876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="9" x14ac:dyDescent="0"/>
@@ -4728,4 +5832,2042 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="13" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="13" customWidth="1"/>
+    <col min="10" max="10" width="3.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" style="12" customWidth="1"/>
+    <col min="12" max="12" width="25.5" style="13" customWidth="1"/>
+    <col min="13" max="16384" width="6.6640625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="20" customFormat="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="11">
+        <v>26</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="G2" s="11">
+        <v>51</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="11">
+        <v>76</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="11">
+        <v>27</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="11">
+        <v>52</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="11">
+        <v>77</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="11">
+        <v>28</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="11">
+        <v>53</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="11">
+        <v>78</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" s="11">
+        <v>29</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" s="11">
+        <v>54</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="11">
+        <v>79</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" s="11">
+        <v>30</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="11">
+        <v>55</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="11">
+        <v>80</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="11">
+        <v>31</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G7" s="11">
+        <v>56</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="11">
+        <v>81</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="13" customFormat="1" ht="44">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D8" s="11">
+        <v>32</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="11">
+        <v>57</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" s="11">
+        <v>82</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="13" customFormat="1" ht="55">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D9" s="11">
+        <v>33</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" s="11">
+        <v>58</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J9" s="11">
+        <v>83</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="13" customFormat="1" ht="44">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D10" s="11">
+        <v>34</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="11">
+        <v>59</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J10" s="11">
+        <v>84</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" s="11">
+        <v>35</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="G11" s="11">
+        <v>60</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" s="11">
+        <v>85</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="D12" s="11">
+        <v>36</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="G12" s="11">
+        <v>61</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="11">
+        <v>86</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="11">
+        <v>37</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="11">
+        <v>62</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="11">
+        <v>87</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="11">
+        <v>38</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" s="11">
+        <v>63</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="J14" s="11">
+        <v>88</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11">
+        <v>39</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="11">
+        <v>64</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="11">
+        <v>89</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="13" customFormat="1" ht="44">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="11">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="G16" s="11">
+        <v>65</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="11">
+        <v>90</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="11">
+        <v>41</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="11">
+        <v>66</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="J17" s="11">
+        <v>91</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="11">
+        <v>42</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="11">
+        <v>67</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" s="11">
+        <v>92</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A19" s="13">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="11">
+        <v>43</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="G19" s="11">
+        <v>68</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="11">
+        <v>93</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A20" s="13">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="11">
+        <v>44</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="11">
+        <v>69</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="J20" s="11">
+        <v>94</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A21" s="13">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="11">
+        <v>45</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="11">
+        <v>70</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" s="11">
+        <v>95</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A22" s="13">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="D22" s="11">
+        <v>46</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G22" s="11">
+        <v>71</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" s="11">
+        <v>96</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A23" s="13">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="11">
+        <v>47</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="11">
+        <v>72</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" s="11">
+        <v>97</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A24" s="13">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="11">
+        <v>48</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="11">
+        <v>73</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="J24" s="11">
+        <v>98</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="13" customFormat="1" ht="33">
+      <c r="A25" s="13">
+        <v>24</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="11">
+        <v>49</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="G25" s="11">
+        <v>74</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="11">
+        <v>99</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="13" customFormat="1" ht="22">
+      <c r="A26" s="13">
+        <v>25</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="11">
+        <v>50</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="11">
+        <v>75</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="11">
+        <v>100</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="A2:L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16" style="13" customWidth="1"/>
+    <col min="4" max="4" width="3.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="3.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="13" customWidth="1"/>
+    <col min="10" max="10" width="3.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="6.6640625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="20" customFormat="1">
+      <c r="A1" s="17"/>
+      <c r="B1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="J1" s="19"/>
+      <c r="K1" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="11">
+        <v>101</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="11">
+        <v>126</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="11">
+        <v>151</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="14">
+        <v>176</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="44">
+      <c r="A3" s="11">
+        <v>102</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="11">
+        <v>127</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="G3" s="11">
+        <v>152</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="14">
+        <v>177</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="22">
+      <c r="A4" s="11">
+        <v>103</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="11">
+        <v>128</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" s="11">
+        <v>153</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="14">
+        <v>178</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="22">
+      <c r="A5" s="11">
+        <v>104</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="D5" s="11">
+        <v>129</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="11">
+        <v>154</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="14">
+        <v>179</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="33">
+      <c r="A6" s="11">
+        <v>105</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="11">
+        <v>130</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="G6" s="11">
+        <v>155</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="14">
+        <v>180</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="22">
+      <c r="A7" s="11">
+        <v>106</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" s="11">
+        <v>131</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="11">
+        <v>156</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="14">
+        <v>181</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="22">
+      <c r="A8" s="11">
+        <v>107</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="11">
+        <v>132</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="G8" s="11">
+        <v>157</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="J8" s="14">
+        <v>182</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="44">
+      <c r="A9" s="11">
+        <v>108</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D9" s="11">
+        <v>133</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="11">
+        <v>158</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="14">
+        <v>183</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="33">
+      <c r="A10" s="11">
+        <v>109</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" s="11">
+        <v>134</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="11">
+        <v>159</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="14">
+        <v>184</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="33">
+      <c r="A11" s="11">
+        <v>110</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" s="11">
+        <v>135</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="G11" s="11">
+        <v>160</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="J11" s="14">
+        <v>185</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="55">
+      <c r="A12" s="11">
+        <v>111</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="11">
+        <v>136</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="11">
+        <v>161</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="J12" s="14">
+        <v>186</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="44">
+      <c r="A13" s="11">
+        <v>112</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="11">
+        <v>137</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="G13" s="11">
+        <v>162</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="J13" s="14">
+        <v>187</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="22">
+      <c r="A14" s="11">
+        <v>113</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="11">
+        <v>138</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="11">
+        <v>163</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="J14" s="14">
+        <v>188</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="33">
+      <c r="A15" s="11">
+        <v>114</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="D15" s="11">
+        <v>139</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="11">
+        <v>164</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" s="14">
+        <v>189</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="22">
+      <c r="A16" s="11">
+        <v>115</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="11">
+        <v>140</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="11">
+        <v>165</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="14">
+        <v>190</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="66">
+      <c r="A17" s="11">
+        <v>116</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="11">
+        <v>141</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="11">
+        <v>166</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J17" s="14">
+        <v>191</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="22">
+      <c r="A18" s="11">
+        <v>117</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="11">
+        <v>142</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="11">
+        <v>167</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="J18" s="14">
+        <v>192</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="33">
+      <c r="A19" s="11">
+        <v>118</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="11">
+        <v>143</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="11">
+        <v>168</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="14">
+        <v>193</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="22">
+      <c r="A20" s="11">
+        <v>119</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11">
+        <v>144</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="11">
+        <v>169</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="J20" s="14">
+        <v>194</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="22">
+      <c r="A21" s="11">
+        <v>120</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="11">
+        <v>145</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="G21" s="11">
+        <v>170</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="14">
+        <v>195</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="11">
+        <v>121</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="11">
+        <v>146</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="11">
+        <v>171</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="J22" s="14">
+        <v>196</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="55">
+      <c r="A23" s="11">
+        <v>122</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="11">
+        <v>147</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="11">
+        <v>172</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="J23" s="14">
+        <v>197</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="11">
+        <v>123</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="11">
+        <v>148</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="11">
+        <v>173</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="J24" s="14">
+        <v>198</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="77">
+      <c r="A25" s="11">
+        <v>124</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="11">
+        <v>149</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="11">
+        <v>174</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="J25" s="14">
+        <v>199</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="33">
+      <c r="A26" s="11">
+        <v>125</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="11">
+        <v>150</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="11">
+        <v>175</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="14">
+        <v>200</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>